<commit_message>
TP#15225 Add signatory and make integration tests pass.
Still need to add the fields to the UI.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\ShipWorks\ShipWorks3x\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ShipWorks\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="462">
   <si>
     <t>SaveLabel</t>
   </si>
@@ -1451,16 +1451,13 @@
   </si>
   <si>
     <t>Re-icing</t>
-  </si>
-  <si>
-    <t>HAZARDOUS_MATERIALS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1535,8 +1532,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1573,8 +1577,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1828,13 +1837,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2001,8 +2026,16 @@
     <xf numFmtId="49" fontId="6" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="3" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 3" xfId="2"/>
     <cellStyle name="Normal 3 10" xfId="1"/>
@@ -2320,10 +2353,10 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:DB83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="CI1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="CH1" sqref="CH1"/>
-      <selection pane="bottomLeft" activeCell="CN101" sqref="CN101"/>
+      <selection pane="bottomLeft" activeCell="CL23" sqref="CL23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7590,9 +7623,7 @@
       <c r="CK23" s="24">
         <v>1</v>
       </c>
-      <c r="CL23" s="24" t="s">
-        <v>462</v>
-      </c>
+      <c r="CL23" s="24"/>
       <c r="CM23" s="24" t="s">
         <v>233</v>
       </c>
@@ -12674,9 +12705,7 @@
       <c r="CK46" s="20">
         <v>0</v>
       </c>
-      <c r="CL46" s="24" t="s">
-        <v>462</v>
-      </c>
+      <c r="CL46" s="24"/>
       <c r="CM46" s="24" t="s">
         <v>233</v>
       </c>
@@ -16672,237 +16701,235 @@
       <c r="DA65" s="31"/>
       <c r="DB65" s="35"/>
     </row>
-    <row r="66" spans="1:106" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:106" s="27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="b">
         <v>1</v>
       </c>
       <c r="B66" s="62"/>
-      <c r="C66" s="36" t="s">
+      <c r="C66" s="64" t="s">
         <v>393</v>
       </c>
-      <c r="D66" s="37" t="s">
+      <c r="D66" s="65" t="s">
         <v>394</v>
       </c>
-      <c r="E66" s="38" t="s">
+      <c r="E66" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="F66" s="31">
+      <c r="F66" s="64">
         <v>323352</v>
       </c>
-      <c r="G66" s="31"/>
-      <c r="H66" s="31" t="s">
+      <c r="G66" s="64"/>
+      <c r="H66" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="I66" s="31" t="s">
+      <c r="I66" s="64" t="s">
         <v>225</v>
       </c>
-      <c r="J66" s="31" t="s">
+      <c r="J66" s="64" t="s">
         <v>155</v>
       </c>
-      <c r="K66" s="36" t="s">
+      <c r="K66" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="L66" s="31">
+      <c r="L66" s="64">
         <v>10</v>
       </c>
-      <c r="M66" s="38" t="s">
+      <c r="M66" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="N66" s="38" t="s">
+      <c r="N66" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="O66" s="36" t="s">
+      <c r="O66" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="P66" s="36" t="s">
+      <c r="P66" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="Q66" s="31" t="s">
+      <c r="Q66" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="R66" s="31" t="s">
+      <c r="R66" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="S66" s="31" t="s">
+      <c r="S66" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="T66" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="U66" s="31"/>
-      <c r="V66" s="36" t="s">
+      <c r="T66" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="U66" s="64"/>
+      <c r="V66" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="W66" s="50" t="s">
+      <c r="W66" s="64" t="s">
         <v>393</v>
       </c>
-      <c r="X66" s="31" t="s">
+      <c r="X66" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="Y66" s="33" t="s">
+      <c r="Y66" s="66" t="s">
         <v>378</v>
       </c>
-      <c r="Z66" s="37" t="s">
+      <c r="Z66" s="65" t="s">
         <v>395</v>
       </c>
-      <c r="AA66" s="31" t="s">
+      <c r="AA66" s="64" t="s">
         <v>217</v>
       </c>
-      <c r="AB66" s="31">
+      <c r="AB66" s="64">
         <v>80002</v>
       </c>
-      <c r="AC66" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="AD66" s="31" t="b">
+      <c r="AC66" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD66" s="64" t="b">
         <v>0</v>
       </c>
-      <c r="AE66" s="31" t="s">
+      <c r="AE66" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="AF66" s="31" t="s">
+      <c r="AF66" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="AG66" s="36" t="s">
+      <c r="AG66" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="AH66" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="AI66" s="31"/>
-      <c r="AJ66" s="31"/>
-      <c r="AK66" s="31"/>
-      <c r="AL66" s="31"/>
-      <c r="AM66" s="31"/>
-      <c r="AN66" s="36"/>
-      <c r="AO66" s="36"/>
-      <c r="AP66" s="36"/>
-      <c r="AQ66" s="36"/>
-      <c r="AR66" s="36"/>
-      <c r="AS66" s="36"/>
-      <c r="AT66" s="36"/>
-      <c r="AU66" s="36"/>
-      <c r="AV66" s="36"/>
-      <c r="AW66" s="36"/>
-      <c r="AX66" s="36"/>
-      <c r="AY66" s="36"/>
-      <c r="AZ66" s="36"/>
-      <c r="BA66" s="36"/>
-      <c r="BB66" s="36"/>
-      <c r="BC66" s="36"/>
-      <c r="BD66" s="36"/>
-      <c r="BE66" s="36"/>
-      <c r="BF66" s="36"/>
-      <c r="BG66" s="36"/>
-      <c r="BH66" s="36"/>
-      <c r="BI66" s="36"/>
-      <c r="BJ66" s="36"/>
-      <c r="BK66" s="38"/>
-      <c r="BL66" s="38"/>
-      <c r="BM66" s="38"/>
-      <c r="BN66" s="38"/>
-      <c r="BO66" s="38"/>
-      <c r="BP66" s="38"/>
-      <c r="BQ66" s="36" t="s">
+      <c r="AH66" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI66" s="64"/>
+      <c r="AJ66" s="64"/>
+      <c r="AK66" s="64"/>
+      <c r="AL66" s="64"/>
+      <c r="AM66" s="64"/>
+      <c r="AN66" s="64"/>
+      <c r="AO66" s="64"/>
+      <c r="AP66" s="64"/>
+      <c r="AQ66" s="64"/>
+      <c r="AR66" s="64"/>
+      <c r="AS66" s="64"/>
+      <c r="AT66" s="64"/>
+      <c r="AU66" s="64"/>
+      <c r="AV66" s="64"/>
+      <c r="AW66" s="64"/>
+      <c r="AX66" s="64"/>
+      <c r="AY66" s="64"/>
+      <c r="AZ66" s="64"/>
+      <c r="BA66" s="64"/>
+      <c r="BB66" s="64"/>
+      <c r="BC66" s="64"/>
+      <c r="BD66" s="64"/>
+      <c r="BE66" s="64"/>
+      <c r="BF66" s="64"/>
+      <c r="BG66" s="64"/>
+      <c r="BH66" s="64"/>
+      <c r="BI66" s="64"/>
+      <c r="BJ66" s="64"/>
+      <c r="BK66" s="66"/>
+      <c r="BL66" s="66"/>
+      <c r="BM66" s="66"/>
+      <c r="BN66" s="66"/>
+      <c r="BO66" s="66"/>
+      <c r="BP66" s="66"/>
+      <c r="BQ66" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="BR66" s="31">
+      <c r="BR66" s="64">
         <v>1</v>
       </c>
-      <c r="BS66" s="31">
+      <c r="BS66" s="64">
         <v>100</v>
       </c>
-      <c r="BT66" s="36" t="s">
+      <c r="BT66" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="BU66" s="36" t="s">
+      <c r="BU66" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="BV66" s="31">
+      <c r="BV66" s="64">
         <v>10</v>
       </c>
-      <c r="BW66" s="31">
+      <c r="BW66" s="64">
         <v>20</v>
       </c>
-      <c r="BX66" s="31">
+      <c r="BX66" s="64">
         <v>15</v>
       </c>
-      <c r="BY66" s="31">
+      <c r="BY66" s="64">
         <v>20</v>
       </c>
-      <c r="BZ66" s="31" t="s">
+      <c r="BZ66" s="64" t="s">
         <v>160</v>
       </c>
-      <c r="CA66" s="36" t="s">
+      <c r="CA66" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="CB66" s="31" t="s">
+      <c r="CB66" s="64" t="s">
         <v>393</v>
       </c>
-      <c r="CC66" s="31" t="s">
+      <c r="CC66" s="64" t="s">
         <v>231</v>
       </c>
-      <c r="CD66" s="31"/>
-      <c r="CE66" s="36"/>
-      <c r="CF66" s="36"/>
-      <c r="CG66" s="36"/>
-      <c r="CH66" s="36"/>
-      <c r="CI66" s="36"/>
-      <c r="CJ66" s="36" t="s">
+      <c r="CD66" s="64"/>
+      <c r="CE66" s="64"/>
+      <c r="CF66" s="64"/>
+      <c r="CG66" s="64"/>
+      <c r="CH66" s="64"/>
+      <c r="CI66" s="64"/>
+      <c r="CJ66" s="64" t="s">
         <v>331</v>
       </c>
-      <c r="CK66" s="36">
+      <c r="CK66" s="64">
         <v>1</v>
       </c>
-      <c r="CL66" s="31" t="s">
-        <v>462</v>
-      </c>
-      <c r="CM66" s="31" t="s">
+      <c r="CL66" s="64"/>
+      <c r="CM66" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="CN66" s="36">
+      <c r="CN66" s="64">
         <v>1</v>
       </c>
-      <c r="CO66" s="36">
+      <c r="CO66" s="64">
         <v>1888</v>
       </c>
-      <c r="CP66" s="36">
+      <c r="CP66" s="64">
         <v>1</v>
       </c>
-      <c r="CQ66" s="36" t="s">
+      <c r="CQ66" s="64" t="s">
         <v>332</v>
       </c>
-      <c r="CR66" s="36">
+      <c r="CR66" s="64">
         <v>1</v>
       </c>
-      <c r="CS66" s="36">
+      <c r="CS66" s="64">
         <v>680</v>
       </c>
-      <c r="CT66" s="31" t="s">
+      <c r="CT66" s="64" t="s">
         <v>333</v>
       </c>
-      <c r="CU66" s="36">
+      <c r="CU66" s="64">
         <v>6.1</v>
       </c>
-      <c r="CV66" s="36">
+      <c r="CV66" s="64">
         <v>1</v>
       </c>
-      <c r="CW66" s="36" t="s">
+      <c r="CW66" s="64" t="s">
         <v>237</v>
       </c>
-      <c r="CX66" s="36" t="s">
+      <c r="CX66" s="64" t="s">
         <v>238</v>
       </c>
-      <c r="CY66" s="36" t="s">
+      <c r="CY66" s="64" t="s">
         <v>239</v>
       </c>
-      <c r="CZ66" s="36" t="s">
+      <c r="CZ66" s="64" t="s">
         <v>240</v>
       </c>
-      <c r="DA66" s="36">
+      <c r="DA66" s="64">
         <v>9015551234</v>
       </c>
-      <c r="DB66" s="35"/>
+      <c r="DB66" s="64"/>
     </row>
     <row r="67" spans="1:106" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="b">
@@ -18168,9 +18195,7 @@
       <c r="CK72" s="31">
         <v>1</v>
       </c>
-      <c r="CL72" s="31" t="s">
-        <v>462</v>
-      </c>
+      <c r="CL72" s="31"/>
       <c r="CM72" s="31" t="s">
         <v>233</v>
       </c>

</xml_diff>

<commit_message>
TP#20088: Fixed manipulators and tests for dangerous goods/batteries/alcohol per cert responses.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Dom.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3775" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3777" uniqueCount="479">
   <si>
     <t>Anchorage</t>
   </si>
@@ -3356,10 +3356,10 @@
   </sheetPr>
   <dimension ref="A1:AQX86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BO1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="DA1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C19" sqref="C19:D19"/>
-      <selection pane="bottomLeft" activeCell="BO38" sqref="BO38"/>
+      <selection pane="bottomLeft" activeCell="DC90" sqref="DC90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -22806,7 +22806,9 @@
       <c r="AH84" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="AI84" s="42"/>
+      <c r="AI84" s="15" t="s">
+        <v>221</v>
+      </c>
       <c r="AJ84" s="42"/>
       <c r="AK84" s="42"/>
       <c r="AL84" s="42" t="s">
@@ -24054,7 +24056,9 @@
       <c r="AH85" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="AI85" s="42"/>
+      <c r="AI85" s="15" t="s">
+        <v>221</v>
+      </c>
       <c r="AJ85" s="42"/>
       <c r="AK85" s="42"/>
       <c r="AL85" s="42" t="s">

</xml_diff>